<commit_message>
base db input addressing organized
</commit_message>
<xml_diff>
--- a/D/iotable.xlsx
+++ b/D/iotable.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EA1382-ECAD-4060-BCDC-17AA0AAFFEC9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
     <sheet name="Output" sheetId="4" r:id="rId2"/>
     <sheet name="Motion" sheetId="5" r:id="rId3"/>
+    <sheet name="SIGNALS" sheetId="6" r:id="rId4"/>
+    <sheet name="CYLINDER SEN A" sheetId="7" r:id="rId5"/>
+    <sheet name="CYLINDER SEN B" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$3:$C$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$4:$C$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Output!$A$3:$C$51</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="115">
   <si>
     <t>Base offset</t>
   </si>
@@ -344,12 +348,33 @@
   </si>
   <si>
     <t>Pnp</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Local offset</t>
+  </si>
+  <si>
+    <t>Abs offset</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -510,6 +535,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -545,6 +587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -720,11 +779,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F67"/>
+      <selection activeCell="E5" sqref="E5:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,22 +792,23 @@
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -756,1394 +816,1683 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3">
+        <v>525231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J4" t="s">
         <v>98</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" ref="E4:E35" si="0">DEC2HEX(B$1*HEX2DEC(1000000)+ MOD(A4,16) * HEX2DEC(10000) + B$2+QUOTIENT(A4,16))</f>
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <f>HEX2DEC(E4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F67" si="1">HEX2DEC(E5)</f>
-        <v>65536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
+        <f>(E5-$B$3)/2</f>
+        <v>-262615.5</v>
+      </c>
+      <c r="H5" t="str">
+        <f>DEC2HEX(B$1*HEX2DEC(1000000)+ G5 + B$2+F5)</f>
+        <v>FBFE28</v>
+      </c>
+      <c r="I5">
+        <f>HEX2DEC(H5)</f>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>20000</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>131072</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6:F69" si="0">(E6-$B$3)/2</f>
+        <v>-262615.5</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H68" si="1">DEC2HEX(B$1*HEX2DEC(1000000)+ G6 + B$2+F6)</f>
+        <v>FBFE28</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I68" si="2">HEX2DEC(H6)</f>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>30000</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>196608</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>40000</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>50000</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>327680</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>60000</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>393216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>70000</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>458752</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>80000</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>524288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>90000</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>589824</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>A0000</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>655360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>B0000</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>720896</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C16">
-        <v>13</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>C0000</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>786432</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C17">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>D0000</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>851968</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>E0000</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>917504</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
         <v>16</v>
       </c>
-      <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>F0000</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>983040</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>16</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>10001</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>65537</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v>20001</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>131073</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>30001</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="1"/>
-        <v>196609</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v>40001</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="1"/>
-        <v>262145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v>50001</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="1"/>
-        <v>327681</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>60001</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="1"/>
-        <v>393217</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v>70001</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
-        <v>458753</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v>80001</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
-        <v>524289</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v>90001</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
-        <v>589825</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v>A0001</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
-        <v>655361</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v>B0001</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="1"/>
-        <v>720897</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C32">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="0"/>
-        <v>C0001</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>786433</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C33">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v>D0001</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="1"/>
-        <v>851969</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C34">
-        <v>15</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>E0001</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="1"/>
-        <v>917505</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>31</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
         <v>16</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>F0001</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
-        <v>983041</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="F36" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+      <c r="L36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>32</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" ref="E36:E67" si="2">DEC2HEX(B$1*HEX2DEC(1000000)+ MOD(A36,16) * HEX2DEC(10000) + B$2+QUOTIENT(A36,16))</f>
-        <v>2</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>33</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" t="str">
-        <f t="shared" si="2"/>
-        <v>10002</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="1"/>
-        <v>65538</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="2"/>
-        <v>20002</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="1"/>
-        <v>131074</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" si="2"/>
-        <v>30002</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="1"/>
-        <v>196610</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C40">
-        <v>5</v>
-      </c>
-      <c r="E40" t="str">
-        <f t="shared" si="2"/>
-        <v>40002</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="1"/>
-        <v>262146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C41">
-        <v>6</v>
-      </c>
-      <c r="E41" t="str">
-        <f t="shared" si="2"/>
-        <v>50002</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="1"/>
-        <v>327682</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C42">
-        <v>7</v>
-      </c>
-      <c r="E42" t="str">
-        <f t="shared" si="2"/>
-        <v>60002</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="1"/>
-        <v>393218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C43">
-        <v>8</v>
-      </c>
-      <c r="E43" t="str">
-        <f t="shared" si="2"/>
-        <v>70002</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="1"/>
-        <v>458754</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C44">
-        <v>9</v>
-      </c>
-      <c r="E44" t="str">
-        <f t="shared" si="2"/>
-        <v>80002</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="1"/>
-        <v>524290</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C45">
-        <v>10</v>
-      </c>
-      <c r="E45" t="str">
-        <f t="shared" si="2"/>
-        <v>90002</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="1"/>
-        <v>589826</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C46">
-        <v>11</v>
-      </c>
-      <c r="E46" t="str">
-        <f t="shared" si="2"/>
-        <v>A0002</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="1"/>
-        <v>655362</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C47">
-        <v>12</v>
-      </c>
-      <c r="E47" t="str">
-        <f t="shared" si="2"/>
-        <v>B0002</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="1"/>
-        <v>720898</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C48">
-        <v>13</v>
-      </c>
-      <c r="E48" t="str">
-        <f t="shared" si="2"/>
-        <v>C0002</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="1"/>
-        <v>786434</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C49">
-        <v>14</v>
-      </c>
-      <c r="E49" t="str">
-        <f t="shared" si="2"/>
-        <v>D0002</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="1"/>
-        <v>851970</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C50">
-        <v>15</v>
-      </c>
-      <c r="E50" t="str">
-        <f t="shared" si="2"/>
-        <v>E0002</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="1"/>
-        <v>917506</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C51">
+        <v>15</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
         <v>16</v>
       </c>
-      <c r="E51" t="str">
-        <f t="shared" si="2"/>
-        <v>F0002</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="1"/>
-        <v>983042</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="F52" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>48</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E52" t="str">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>49</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="E53" t="str">
-        <f t="shared" si="2"/>
-        <v>10003</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="1"/>
-        <v>65539</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="E54" t="str">
-        <f t="shared" si="2"/>
-        <v>20003</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="1"/>
-        <v>131075</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C55">
-        <v>4</v>
-      </c>
-      <c r="E55" t="str">
-        <f t="shared" si="2"/>
-        <v>30003</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="1"/>
-        <v>196611</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C56">
-        <v>5</v>
-      </c>
-      <c r="E56" t="str">
-        <f t="shared" si="2"/>
-        <v>40003</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="1"/>
-        <v>262147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C57">
-        <v>6</v>
-      </c>
-      <c r="E57" t="str">
-        <f t="shared" si="2"/>
-        <v>50003</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="1"/>
-        <v>327683</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C58">
-        <v>7</v>
-      </c>
-      <c r="E58" t="str">
-        <f t="shared" si="2"/>
-        <v>60003</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="1"/>
-        <v>393219</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C59">
-        <v>8</v>
-      </c>
-      <c r="E59" t="str">
-        <f t="shared" si="2"/>
-        <v>70003</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="1"/>
-        <v>458755</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C60">
-        <v>9</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" t="str">
-        <f t="shared" si="2"/>
-        <v>80003</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="1"/>
-        <v>524291</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C61">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E61" t="str">
-        <f t="shared" si="2"/>
-        <v>90003</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="1"/>
-        <v>589827</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C62">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" t="str">
-        <f t="shared" si="2"/>
-        <v>A0003</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="1"/>
-        <v>655363</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C63">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E63" t="str">
-        <f t="shared" si="2"/>
-        <v>B0003</v>
-      </c>
-      <c r="F63">
-        <f t="shared" si="1"/>
-        <v>720899</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C64">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E64" t="str">
-        <f t="shared" si="2"/>
-        <v>C0003</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="1"/>
-        <v>786435</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C65">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E65" t="str">
-        <f t="shared" si="2"/>
-        <v>D0003</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="1"/>
-        <v>851971</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C66">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E66" t="str">
-        <f t="shared" si="2"/>
-        <v>E0003</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="1"/>
-        <v>917507</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C67">
+        <v>15</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>63</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68">
         <v>16</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E67" t="str">
-        <f t="shared" si="2"/>
-        <v>F0003</v>
-      </c>
-      <c r="F67">
-        <f t="shared" si="1"/>
-        <v>983043</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="1"/>
+        <v>FBFE28</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="2"/>
+        <v>16514600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="1">
+        <f t="shared" si="0"/>
+        <v>-262615.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="1">
+        <f t="shared" ref="F70:F72" si="3">(E70-$B$3)/2</f>
+        <v>-262615.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F71" s="1">
+        <f t="shared" si="3"/>
+        <v>-262615.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B72" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="3"/>
+        <v>-262615.5</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C67"/>
+  <autoFilter ref="A4:C68" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -3255,17 +3604,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C51"/>
+  <autoFilter ref="A3:C51" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3320,4 +3669,543 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69CFC3F-26AD-4FF9-8B91-56700D135D7F}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1">
+        <v>525231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f>$B$1+A4*$B$2</f>
+        <v>525231</v>
+      </c>
+      <c r="C4">
+        <f>A4*$B$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B14" si="0">$B$1+A5*$B$2</f>
+        <v>525311</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C14" si="1">A5*$B$2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>525391</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>525471</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>525551</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>525631</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>525711</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>525791</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>525871</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>525951</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>526031</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AD2CBD-F75F-4320-8EF3-6C46AE9359C1}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" activeCellId="5" sqref="B5 B8 B9 B10 B18 B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1">
+        <v>530284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f>$B$1+A4*$B$2</f>
+        <v>530284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B19" si="0">$B$1+A5*$B$2</f>
+        <v>530420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>530556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>530692</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>530828</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>530964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>531100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>531236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>531372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>531508</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>531644</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>531780</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>531916</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>532052</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>532188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>532324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBD1E14-95B0-42A9-B01D-B8348254E65B}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" activeCellId="2" sqref="B16 B18 B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1">
+        <v>530288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f>$B$1+A4*$B$2</f>
+        <v>530288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B19" si="0">$B$1+A5*$B$2</f>
+        <v>530424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>530560</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>530696</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>530832</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>530968</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>531104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>531240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>531376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>531512</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>531648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>531784</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>531920</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>532056</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>532192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>532328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>